<commit_message>
vault backup: 2025-05-22 21:00:07
</commit_message>
<xml_diff>
--- a/de/fpu/include_f16mis/fmis_round.xlsx
+++ b/de/fpu/include_f16mis/fmis_round.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\obs\de\fpu\include_f16mis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DF4F0E0-9424-48EA-861B-2E78537BB8FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC419011-3330-4DA7-ABB5-73C403825922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="29676" windowHeight="17496" xr2:uid="{2D388918-9C0E-4326-B0D2-841977531A06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>Sign</t>
   </si>
@@ -122,20 +123,81 @@
     <t>Floating-point to negative integer</t>
   </si>
   <si>
-    <t>convert then rouding</t>
-  </si>
-  <si>
     <t>rounding</t>
   </si>
   <si>
-    <t>rounding then convert</t>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>r_inc</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0001</t>
+  </si>
+  <si>
+    <t>-2</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0010</t>
+  </si>
+  <si>
+    <t>-1 with 2comp become pos</t>
+  </si>
+  <si>
+    <t>result with 2 comp become neg</t>
+  </si>
+  <si>
+    <t>1 comp</t>
+  </si>
+  <si>
+    <t>1110</t>
+  </si>
+  <si>
+    <t>1111 (-1)</t>
+  </si>
+  <si>
+    <t>1110 (-2)</t>
+  </si>
+  <si>
+    <t>final result</t>
+  </si>
+  <si>
+    <t>1110 + 1</t>
+  </si>
+  <si>
+    <t>1101 + 1</t>
+  </si>
+  <si>
+    <t>rounding then convert2neg</t>
+  </si>
+  <si>
+    <t>conver2pos then rouding</t>
+  </si>
+  <si>
+    <t>fast convert2neg algorithm</t>
+  </si>
+  <si>
+    <t>slow convert2neg algorithm</t>
+  </si>
+  <si>
+    <t>這個algorithm可以減少一個ADD
+注意r_inc的行爲與原演算法相反</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,8 +219,23 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,6 +245,17 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -195,11 +283,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -217,18 +306,27 @@
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -563,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07FC8797-3C55-4DEA-B656-0951CF4FDAC3}">
   <dimension ref="C4:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -942,12 +1040,6 @@
       <c r="M14" s="3">
         <v>1</v>
       </c>
-      <c r="O14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="P14" s="9" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D15" s="1">
@@ -980,12 +1072,6 @@
       <c r="M15" s="3">
         <v>1</v>
       </c>
-      <c r="O15" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="P15" s="9" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="16" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D16" s="1">
@@ -1018,14 +1104,8 @@
       <c r="M16" s="3">
         <v>1</v>
       </c>
-      <c r="O16" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="P16" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="4:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D17" s="1">
         <v>1</v>
       </c>
@@ -1056,14 +1136,8 @@
       <c r="M17" s="3">
         <v>1</v>
       </c>
-      <c r="O17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="P17" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="4:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D18" s="1">
         <v>1</v>
       </c>
@@ -1095,7 +1169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D19" s="1">
         <v>1</v>
       </c>
@@ -1127,7 +1201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D20" s="1">
         <v>1</v>
       </c>
@@ -1159,7 +1233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D21" s="1">
         <v>1</v>
       </c>
@@ -1191,11 +1265,278 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:15" x14ac:dyDescent="0.3">
       <c r="O24" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC87B18-E3D2-4ACE-AEAB-BFA350FB7D58}">
+  <dimension ref="D2:N20"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="H2" s="9"/>
+    </row>
+    <row r="4" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+    </row>
+    <row r="9" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+    </row>
+    <row r="12" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+    </row>
+    <row r="13" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="9"/>
+    </row>
+    <row r="14" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="9"/>
+      <c r="H14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="M14" s="9"/>
+    </row>
+    <row r="15" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="H17" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+    </row>
+    <row r="18" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G18" s="9"/>
+      <c r="H18" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="L18" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+    </row>
+    <row r="19" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G19" s="9"/>
+      <c r="H19" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K19" s="12"/>
+      <c r="L19" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+    </row>
+    <row r="20" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G20" s="9"/>
+      <c r="H20" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K20" s="12"/>
+      <c r="L20" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="K18:K20"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="H13:L13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
vault backup: 2025-05-23 16:03:02
</commit_message>
<xml_diff>
--- a/de/fpu/include_f16mis/fmis_round.xlsx
+++ b/de/fpu/include_f16mis/fmis_round.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\obs\de\fpu\include_f16mis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC419011-3330-4DA7-ABB5-73C403825922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612CEECA-B68A-439F-9B31-CCF197778393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="29676" windowHeight="17496" xr2:uid="{2D388918-9C0E-4326-B0D2-841977531A06}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="29676" windowHeight="17496" activeTab="1" xr2:uid="{2D388918-9C0E-4326-B0D2-841977531A06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,14 +183,14 @@
     <t>conver2pos then rouding</t>
   </si>
   <si>
-    <t>fast convert2neg algorithm</t>
-  </si>
-  <si>
-    <t>slow convert2neg algorithm</t>
-  </si>
-  <si>
     <t>這個algorithm可以減少一個ADD
 注意r_inc的行爲與原演算法相反</t>
+  </si>
+  <si>
+    <t>slow rounding_then_convert2neg</t>
+  </si>
+  <si>
+    <t>fast rounding_then_convert2neg</t>
   </si>
 </sst>
 </file>
@@ -313,15 +313,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -661,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07FC8797-3C55-4DEA-B656-0951CF4FDAC3}">
   <dimension ref="C4:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1278,8 +1278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC87B18-E3D2-4ACE-AEAB-BFA350FB7D58}">
   <dimension ref="D2:N20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1384,13 +1384,13 @@
         <v>27</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
       <c r="M13" s="9"/>
     </row>
     <row r="14" spans="4:13" x14ac:dyDescent="0.3">
@@ -1401,19 +1401,19 @@
         <v>46</v>
       </c>
       <c r="G14" s="9"/>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="J14" s="11" t="s">
+      <c r="J14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="K14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="L14" s="11" t="s">
+      <c r="L14" s="10" t="s">
         <v>42</v>
       </c>
       <c r="M14" s="9"/>
@@ -1426,19 +1426,19 @@
         <v>27</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="I15" s="11" t="s">
+      <c r="I15" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="J15" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K15" s="11" t="s">
+      <c r="K15" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="L15" s="11" t="s">
+      <c r="L15" s="10" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1450,46 +1450,46 @@
         <v>45</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J16" s="11" t="s">
+      <c r="J16" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="11" t="s">
+      <c r="K16" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="L16" s="11" t="s">
+      <c r="L16" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="7:14" x14ac:dyDescent="0.3">
-      <c r="H17" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
+      <c r="H17" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
     </row>
     <row r="18" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G18" s="9"/>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="J18" s="11" t="s">
+      <c r="J18" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="L18" s="11" t="s">
+      <c r="K18" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="L18" s="10" t="s">
         <v>42</v>
       </c>
       <c r="M18" s="9"/>
@@ -1497,17 +1497,17 @@
     </row>
     <row r="19" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G19" s="9"/>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J19" s="11" t="s">
+      <c r="J19" s="10" t="s">
         <v>30</v>
       </c>
       <c r="K19" s="12"/>
-      <c r="L19" s="11" t="s">
+      <c r="L19" s="10" t="s">
         <v>40</v>
       </c>
       <c r="M19" s="9"/>
@@ -1515,17 +1515,17 @@
     </row>
     <row r="20" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G20" s="9"/>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J20" s="11" t="s">
+      <c r="J20" s="10" t="s">
         <v>31</v>
       </c>
       <c r="K20" s="12"/>
-      <c r="L20" s="11" t="s">
+      <c r="L20" s="10" t="s">
         <v>41</v>
       </c>
       <c r="M20" s="9"/>

</xml_diff>